<commit_message>
Finalize restoration biomass change calculation.
</commit_message>
<xml_diff>
--- a/LDMP/data/summary_table_restoration.xlsx
+++ b/LDMP/data/summary_table_restoration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azvol\Code\LandDegradation\trends.earth\LDMP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02842FD8-41B5-4CBE-8397-C7FF820F4117}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71670B3D-5673-4BFA-8F04-48DF25EDFFDD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -313,56 +313,56 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -696,10 +696,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,83 +712,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="36"/>
+      <c r="B1" s="32"/>
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:4" s="11" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
     </row>
     <row r="4" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
     </row>
     <row r="5" spans="1:4" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="33" t="s">
+      <c r="A5" s="26"/>
+      <c r="B5" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="31"/>
+      <c r="D5" s="25"/>
     </row>
     <row r="6" spans="1:4" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="22">
         <v>0</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="35"/>
+      <c r="D6" s="29"/>
     </row>
     <row r="7" spans="1:4" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="22">
         <v>15</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="35"/>
+      <c r="D7" s="29"/>
     </row>
     <row r="8" spans="1:4" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="28">
+      <c r="B8" s="22">
         <v>55646123</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="35"/>
+      <c r="D8" s="29"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
     </row>
     <row r="10" spans="1:4" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
     </row>
     <row r="11" spans="1:4" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
@@ -816,47 +816,46 @@
       <c r="C14" s="14"/>
       <c r="D14" s="10"/>
     </row>
-    <row r="15" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-    </row>
-    <row r="16" spans="1:4" s="9" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+    </row>
+    <row r="16" spans="1:4" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-    </row>
-    <row r="17" spans="1:3" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+    </row>
+    <row r="17" spans="1:3" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="1:3" s="5" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
+    <row r="18" spans="1:3" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+    </row>
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-    </row>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+    </row>
+    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A18:C18"/>
     <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A16:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="84" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix calculation of change, and include total biomass in sheet.
</commit_message>
<xml_diff>
--- a/LDMP/data/summary_table_restoration.xlsx
+++ b/LDMP/data/summary_table_restoration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azvol\Code\LandDegradation\trends.earth\LDMP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71670B3D-5673-4BFA-8F04-48DF25EDFFDD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573EFAA7-7166-42F0-BE41-1E0DC0CC481D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>The boundaries, names, and designations used in this report do not imply official endorsement or acceptance by Conservation International Foundation, or its partner organizations and contributors.  This report is available under the terms of Creative Commons Attribution 4.0 International License (CC BY 4.0).</t>
   </si>
@@ -128,6 +128,35 @@
   </si>
   <si>
     <t>Change in biomass with restoration</t>
+  </si>
+  <si>
+    <r>
+      <t>Final total biomass
+(tonnes CO</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>e)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -699,7 +728,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,7 +802,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="22">
-        <v>55646123</v>
+        <v>0</v>
       </c>
       <c r="C8" s="24" t="s">
         <v>8</v>
@@ -802,11 +831,16 @@
       <c r="B12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="12"/>
+      <c r="C12" s="15" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="13" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="18">
+        <v>0</v>
+      </c>
+      <c r="C13" s="18">
         <v>0</v>
       </c>
     </row>

</xml_diff>